<commit_message>
fix issues for client
</commit_message>
<xml_diff>
--- a/client/public/assets/student_import_template.xlsx
+++ b/client/public/assets/student_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akramjaouni/Desktop/Repos/AcademicTeamManagement/client/public/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B00D93F-F058-2046-AE97-B87E16EB0029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6497E1F4-B09E-0447-896F-1318966C73C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>OrgDefinedId</t>
   </si>
@@ -52,19 +52,10 @@
     <t>Sections</t>
   </si>
   <si>
-    <t>Calculated Final Grade Numerator</t>
+    <t>End-of-Line Indicator</t>
   </si>
   <si>
-    <t>Calculated Final Grade Denominator</t>
-  </si>
-  <si>
-    <t>Adjusted Final Grade Numerator</t>
-  </si>
-  <si>
-    <t>Adjusted Final Grade Denominator</t>
-  </si>
-  <si>
-    <t>End-of-Line Indicator</t>
+    <t>Final grade</t>
   </si>
 </sst>
 </file>
@@ -578,11 +569,10 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -939,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -954,89 +944,43 @@
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="22.1640625" customWidth="1"/>
     <col min="7" max="7" width="27.83203125" customWidth="1"/>
-    <col min="8" max="8" width="29" customWidth="1"/>
-    <col min="9" max="9" width="26.83203125" customWidth="1"/>
-    <col min="10" max="10" width="28.1640625" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>